<commit_message>
Added Yidan's timesheet for week7-12
</commit_message>
<xml_diff>
--- a/Timesheet/Timesheet_Week2-6_YidanWang.xlsx
+++ b/Timesheet/Timesheet_Week2-6_YidanWang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yidanwang/Desktop/MCIP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yidanwang/Desktop/MCIP/Team-17E/Timesheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A33BE5A-BB1F-A241-BA3B-DF4B8F284969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3761DFC-F0B9-B641-A188-C9EECE3359EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="1400" windowWidth="27640" windowHeight="16780" activeTab="4" xr2:uid="{CB0E90D9-F2E7-6C41-904C-336099D9E1F5}"/>
+    <workbookView xWindow="2600" yWindow="1320" windowWidth="27640" windowHeight="16780" xr2:uid="{CB0E90D9-F2E7-6C41-904C-336099D9E1F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Week2" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Week5" sheetId="4" r:id="rId4"/>
     <sheet name="Week6" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t>Get better user experience</t>
+  </si>
+  <si>
+    <t>Week starting: Week6</t>
+  </si>
+  <si>
+    <t>Week starting: Week5</t>
+  </si>
+  <si>
+    <t>Week starting: Week4</t>
+  </si>
+  <si>
+    <t>Week starting: Week3</t>
   </si>
 </sst>
 </file>
@@ -228,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -519,7 +531,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -537,7 +549,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -555,22 +567,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -586,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,10 +601,10 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -610,6 +616,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -948,23 +960,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAD620A-71DA-FD42-BDDB-D3AB98BBB978}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1175,22 +1187,22 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1204,170 +1216,170 @@
       <c r="E2" s="3"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="30">
         <v>3.11</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="32">
         <v>6</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="30">
         <v>3.12</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="34">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="34">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>6</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="30">
         <v>3.13</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="31">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="31">
         <v>0.75</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>8</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="30">
         <v>3.14</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>6</v>
       </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="30">
         <v>3.15</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="31">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>4</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="32"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="36">
         <f>SUM(E5:E10)</f>
         <v>30</v>
       </c>
@@ -1391,22 +1403,22 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1420,170 +1432,170 @@
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>3.18</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>6</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>3.19</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="34">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="34">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>6</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="37">
         <v>3.2</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="31">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="31">
         <v>0.75</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>8</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>3.21</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>6</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="37">
         <v>3.22</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="31">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>4</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="32"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="36">
         <f>SUM(E6:E11)</f>
         <v>30</v>
       </c>
@@ -1607,7 +1619,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1616,16 +1628,16 @@
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1639,7 +1651,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="H3" s="18"/>
     </row>
@@ -1647,172 +1659,172 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="30">
         <v>3.25</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>6</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="39" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="30">
         <v>3.26</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="34">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="34">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>6</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="30">
         <v>3.27</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="31">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="31">
         <v>0.75</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>8</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="39" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="30">
         <v>3.28</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>6</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="39" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="30">
         <v>3.29</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="31">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>4</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="41"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="41"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="36">
         <f>SUM(E6:E11)</f>
         <v>30</v>
       </c>
@@ -1836,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6DA19A-18B2-994D-8F11-5E64310F8435}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1853,16 +1865,16 @@
       <c r="H1" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1876,170 +1888,170 @@
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="4" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="30">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>6</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="30">
         <v>4.2</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="34">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="34">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>6</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="30">
         <v>4.3</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="31">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="31">
         <v>0.75</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>8</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="30">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="31">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>6</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="30">
         <v>4.5</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="31">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="31">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="32">
         <v>4</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="32"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="36">
         <f>SUM(E7:E12)</f>
         <v>30</v>
       </c>

</xml_diff>